<commit_message>
Updated result spreadsheets and script for manual analysis
</commit_message>
<xml_diff>
--- a/datasets_info/fidelity_experiments/fidelity_movies.xlsx
+++ b/datasets_info/fidelity_experiments/fidelity_movies.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25330"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25427"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mentos\Documents\Studia\Semestr 10\Magisterka\peter\PETER\datasets_info\fidelity_experiments\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B81485EB-7FBD-4249-9320-8A5663571714}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C29692A9-BD69-498D-883E-2A21DCAC2766}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13065" yWindow="1275" windowWidth="12735" windowHeight="12975" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="11910" yWindow="1035" windowWidth="15615" windowHeight="12975" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Arkusz1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="15">
   <si>
     <t>GT dobre [1,5]</t>
   </si>
@@ -69,6 +69,15 @@
   </si>
   <si>
     <t>Predykcje spójne</t>
+  </si>
+  <si>
+    <t>Podwójny recommender</t>
+  </si>
+  <si>
+    <t>Predykcja spójna</t>
+  </si>
+  <si>
+    <t>Rating input</t>
   </si>
 </sst>
 </file>
@@ -113,13 +122,17 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normalny" xfId="0" builtinId="0"/>
@@ -400,10 +413,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L102"/>
+  <dimension ref="A1:AD102"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+    <sheetView tabSelected="1" topLeftCell="U1" workbookViewId="0">
+      <selection activeCell="AC5" sqref="AC5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -415,9 +428,17 @@
     <col min="7" max="7" width="18.28515625" customWidth="1"/>
     <col min="11" max="11" width="22.85546875" customWidth="1"/>
     <col min="12" max="12" width="18.28515625" customWidth="1"/>
+    <col min="15" max="15" width="20" customWidth="1"/>
+    <col min="16" max="16" width="24.28515625" customWidth="1"/>
+    <col min="17" max="17" width="18" customWidth="1"/>
+    <col min="20" max="20" width="13.42578125" customWidth="1"/>
+    <col min="21" max="21" width="17.85546875" customWidth="1"/>
+    <col min="24" max="24" width="15.7109375" customWidth="1"/>
+    <col min="25" max="25" width="11.42578125" customWidth="1"/>
+    <col min="29" max="29" width="16.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:30" x14ac:dyDescent="0.25">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -436,11 +457,39 @@
       <c r="G1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="O1" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="P1" s="5"/>
+      <c r="Q1" s="5"/>
+      <c r="X1" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="Y1" s="5"/>
+      <c r="Z1" s="5"/>
+    </row>
+    <row r="2" spans="1:30" x14ac:dyDescent="0.25">
       <c r="G2" s="2"/>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="O2" t="s">
+        <v>13</v>
+      </c>
+      <c r="P2" t="s">
+        <v>8</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>9</v>
+      </c>
+      <c r="X2" t="s">
+        <v>13</v>
+      </c>
+      <c r="Y2" t="s">
+        <v>8</v>
+      </c>
+      <c r="Z2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1385</v>
       </c>
@@ -451,7 +500,7 @@
         <v>1</v>
       </c>
       <c r="D3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E3">
         <v>4</v>
@@ -462,8 +511,20 @@
       <c r="K3" s="3" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="N3">
+        <v>1385</v>
+      </c>
+      <c r="O3">
+        <v>0</v>
+      </c>
+      <c r="W3">
+        <v>1385</v>
+      </c>
+      <c r="X3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2269</v>
       </c>
@@ -482,8 +543,20 @@
       <c r="F4">
         <v>5</v>
       </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="N4">
+        <v>2269</v>
+      </c>
+      <c r="O4">
+        <v>1</v>
+      </c>
+      <c r="W4">
+        <v>2269</v>
+      </c>
+      <c r="X4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>6613</v>
       </c>
@@ -513,8 +586,27 @@
       <c r="L5" s="3" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="N5">
+        <v>6613</v>
+      </c>
+      <c r="O5">
+        <v>0</v>
+      </c>
+      <c r="S5" s="4"/>
+      <c r="T5" s="4"/>
+      <c r="U5" s="4"/>
+      <c r="V5" s="4"/>
+      <c r="W5">
+        <v>6613</v>
+      </c>
+      <c r="X5">
+        <v>1</v>
+      </c>
+      <c r="AB5" s="4"/>
+      <c r="AC5" s="4"/>
+      <c r="AD5" s="4"/>
+    </row>
+    <row r="6" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>6697</v>
       </c>
@@ -525,7 +617,7 @@
         <v>0</v>
       </c>
       <c r="D6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E6">
         <v>1</v>
@@ -548,8 +640,27 @@
         <f>COUNTIF($F$3:$F$102,I6)</f>
         <v>18</v>
       </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="N6">
+        <v>6697</v>
+      </c>
+      <c r="O6">
+        <v>0</v>
+      </c>
+      <c r="S6" s="4"/>
+      <c r="T6" s="4"/>
+      <c r="U6" s="4"/>
+      <c r="V6" s="4"/>
+      <c r="W6">
+        <v>6697</v>
+      </c>
+      <c r="X6">
+        <v>0</v>
+      </c>
+      <c r="AB6" s="4"/>
+      <c r="AC6" s="4"/>
+      <c r="AD6" s="4"/>
+    </row>
+    <row r="7" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>10365</v>
       </c>
@@ -583,8 +694,27 @@
         <f>COUNTIF($F$3:$F$102,I7)</f>
         <v>35</v>
       </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="N7">
+        <v>10365</v>
+      </c>
+      <c r="O7">
+        <v>1</v>
+      </c>
+      <c r="S7" s="4"/>
+      <c r="T7" s="4"/>
+      <c r="U7" s="4"/>
+      <c r="V7" s="4"/>
+      <c r="W7">
+        <v>10365</v>
+      </c>
+      <c r="X7">
+        <v>1</v>
+      </c>
+      <c r="AB7" s="4"/>
+      <c r="AC7" s="4"/>
+      <c r="AD7" s="4"/>
+    </row>
+    <row r="8" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>11501</v>
       </c>
@@ -618,8 +748,27 @@
         <f>COUNTIF($F$3:$F$102,I8)</f>
         <v>10</v>
       </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="N8">
+        <v>11501</v>
+      </c>
+      <c r="O8">
+        <v>1</v>
+      </c>
+      <c r="S8" s="4"/>
+      <c r="T8" s="4"/>
+      <c r="U8" s="4"/>
+      <c r="V8" s="4"/>
+      <c r="W8">
+        <v>11501</v>
+      </c>
+      <c r="X8">
+        <v>1</v>
+      </c>
+      <c r="AB8" s="4"/>
+      <c r="AC8" s="4"/>
+      <c r="AD8" s="4"/>
+    </row>
+    <row r="9" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>16385</v>
       </c>
@@ -653,8 +802,27 @@
         <f>COUNTIF($F$3:$F$102,I9)</f>
         <v>15</v>
       </c>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="N9">
+        <v>16385</v>
+      </c>
+      <c r="O9">
+        <v>1</v>
+      </c>
+      <c r="S9" s="4"/>
+      <c r="T9" s="4"/>
+      <c r="U9" s="4"/>
+      <c r="V9" s="4"/>
+      <c r="W9">
+        <v>16385</v>
+      </c>
+      <c r="X9">
+        <v>0</v>
+      </c>
+      <c r="AB9" s="4"/>
+      <c r="AC9" s="4"/>
+      <c r="AD9" s="4"/>
+    </row>
+    <row r="10" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>20737</v>
       </c>
@@ -688,8 +856,31 @@
         <f>COUNTIF($F$3:$F$102,I10)</f>
         <v>21</v>
       </c>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="N10">
+        <v>20737</v>
+      </c>
+      <c r="O10">
+        <v>1</v>
+      </c>
+      <c r="S10" s="4"/>
+      <c r="T10" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="U10" s="4"/>
+      <c r="V10" s="4"/>
+      <c r="W10">
+        <v>20737</v>
+      </c>
+      <c r="X10">
+        <v>1</v>
+      </c>
+      <c r="AB10" s="4"/>
+      <c r="AC10" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="AD10" s="4"/>
+    </row>
+    <row r="11" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>22821</v>
       </c>
@@ -708,8 +899,27 @@
       <c r="F11">
         <v>2</v>
       </c>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="N11">
+        <v>22821</v>
+      </c>
+      <c r="O11">
+        <v>0</v>
+      </c>
+      <c r="S11" s="4"/>
+      <c r="T11" s="4"/>
+      <c r="U11" s="4"/>
+      <c r="V11" s="4"/>
+      <c r="W11">
+        <v>22821</v>
+      </c>
+      <c r="X11">
+        <v>0</v>
+      </c>
+      <c r="AB11" s="4"/>
+      <c r="AC11" s="4"/>
+      <c r="AD11" s="4"/>
+    </row>
+    <row r="12" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>23157</v>
       </c>
@@ -735,8 +945,34 @@
       <c r="K12" s="3" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="N12">
+        <v>23157</v>
+      </c>
+      <c r="O12">
+        <v>1</v>
+      </c>
+      <c r="S12" s="3"/>
+      <c r="T12" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="U12" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="W12">
+        <v>23157</v>
+      </c>
+      <c r="X12">
+        <v>1</v>
+      </c>
+      <c r="AB12" s="3"/>
+      <c r="AC12" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="AD12" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>23161</v>
       </c>
@@ -764,10 +1000,44 @@
       </c>
       <c r="K13" s="3">
         <f t="shared" si="0"/>
+        <v>43</v>
+      </c>
+      <c r="N13">
+        <v>23161</v>
+      </c>
+      <c r="O13">
+        <v>0</v>
+      </c>
+      <c r="S13" s="3">
+        <v>0</v>
+      </c>
+      <c r="T13" s="3">
+        <f>COUNTIF(C$3:C$102,$S13)</f>
+        <v>34</v>
+      </c>
+      <c r="U13" s="3">
+        <f>COUNTIF(O$3:O$102,$S13)</f>
         <v>42</v>
       </c>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="W13">
+        <v>23161</v>
+      </c>
+      <c r="X13">
+        <v>0</v>
+      </c>
+      <c r="AB13" s="3">
+        <v>0</v>
+      </c>
+      <c r="AC13" s="3">
+        <f>COUNTIF(L$3:L$102,$S13)</f>
+        <v>0</v>
+      </c>
+      <c r="AD13" s="3">
+        <f>COUNTIF(X$3:X$102,$S13)</f>
+        <v>48</v>
+      </c>
+    </row>
+    <row r="14" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>27613</v>
       </c>
@@ -797,8 +1067,42 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="N14">
+        <v>27613</v>
+      </c>
+      <c r="O14">
+        <v>0</v>
+      </c>
+      <c r="S14" s="3">
+        <v>1</v>
+      </c>
+      <c r="T14" s="3">
+        <f>COUNTIF(C$3:C$102,$S14)</f>
+        <v>66</v>
+      </c>
+      <c r="U14" s="3">
+        <f>COUNTIF(O$3:O$102,$S14)</f>
+        <v>58</v>
+      </c>
+      <c r="W14">
+        <v>27613</v>
+      </c>
+      <c r="X14">
+        <v>0</v>
+      </c>
+      <c r="AB14" s="3">
+        <v>1</v>
+      </c>
+      <c r="AC14" s="3">
+        <f>COUNTIF(L$3:L$102,$S14)</f>
+        <v>0</v>
+      </c>
+      <c r="AD14" s="3">
+        <f>COUNTIF(X$3:X$102,$S14)</f>
+        <v>52</v>
+      </c>
+    </row>
+    <row r="15" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>30009</v>
       </c>
@@ -826,10 +1130,28 @@
       </c>
       <c r="K15" s="3">
         <f t="shared" si="0"/>
-        <v>58</v>
-      </c>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+        <v>57</v>
+      </c>
+      <c r="N15">
+        <v>30009</v>
+      </c>
+      <c r="O15">
+        <v>1</v>
+      </c>
+      <c r="S15" s="4"/>
+      <c r="T15" s="4"/>
+      <c r="U15" s="4"/>
+      <c r="W15">
+        <v>30009</v>
+      </c>
+      <c r="X15">
+        <v>0</v>
+      </c>
+      <c r="AB15" s="4"/>
+      <c r="AC15" s="4"/>
+      <c r="AD15" s="4"/>
+    </row>
+    <row r="16" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>34201</v>
       </c>
@@ -848,8 +1170,20 @@
       <c r="F16">
         <v>2</v>
       </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="N16">
+        <v>34201</v>
+      </c>
+      <c r="O16">
+        <v>0</v>
+      </c>
+      <c r="W16">
+        <v>34201</v>
+      </c>
+      <c r="X16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>37461</v>
       </c>
@@ -868,8 +1202,20 @@
       <c r="F17">
         <v>1</v>
       </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="N17">
+        <v>37461</v>
+      </c>
+      <c r="O17">
+        <v>1</v>
+      </c>
+      <c r="W17">
+        <v>37461</v>
+      </c>
+      <c r="X17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>38581</v>
       </c>
@@ -888,8 +1234,20 @@
       <c r="F18">
         <v>4</v>
       </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="N18">
+        <v>38581</v>
+      </c>
+      <c r="O18">
+        <v>0</v>
+      </c>
+      <c r="W18">
+        <v>38581</v>
+      </c>
+      <c r="X18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>40761</v>
       </c>
@@ -908,8 +1266,20 @@
       <c r="F19">
         <v>5</v>
       </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="N19">
+        <v>40761</v>
+      </c>
+      <c r="O19">
+        <v>1</v>
+      </c>
+      <c r="W19">
+        <v>40761</v>
+      </c>
+      <c r="X19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>41161</v>
       </c>
@@ -920,7 +1290,7 @@
         <v>0</v>
       </c>
       <c r="D20">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E20">
         <v>1</v>
@@ -928,8 +1298,20 @@
       <c r="F20">
         <v>3</v>
       </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="N20">
+        <v>41161</v>
+      </c>
+      <c r="O20">
+        <v>0</v>
+      </c>
+      <c r="W20">
+        <v>41161</v>
+      </c>
+      <c r="X20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>41437</v>
       </c>
@@ -948,8 +1330,20 @@
       <c r="F21">
         <v>5</v>
       </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="N21">
+        <v>41437</v>
+      </c>
+      <c r="O21">
+        <v>1</v>
+      </c>
+      <c r="W21">
+        <v>41437</v>
+      </c>
+      <c r="X21">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>43113</v>
       </c>
@@ -968,8 +1362,20 @@
       <c r="F22">
         <v>2</v>
       </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="N22">
+        <v>43113</v>
+      </c>
+      <c r="O22">
+        <v>0</v>
+      </c>
+      <c r="W22">
+        <v>43113</v>
+      </c>
+      <c r="X22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>45457</v>
       </c>
@@ -988,8 +1394,20 @@
       <c r="F23">
         <v>2</v>
       </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="N23">
+        <v>45457</v>
+      </c>
+      <c r="O23">
+        <v>1</v>
+      </c>
+      <c r="W23">
+        <v>45457</v>
+      </c>
+      <c r="X23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>46833</v>
       </c>
@@ -1008,8 +1426,20 @@
       <c r="F24">
         <v>4</v>
       </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="N24">
+        <v>46833</v>
+      </c>
+      <c r="O24">
+        <v>1</v>
+      </c>
+      <c r="W24">
+        <v>46833</v>
+      </c>
+      <c r="X24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>47505</v>
       </c>
@@ -1028,8 +1458,20 @@
       <c r="F25">
         <v>5</v>
       </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="N25">
+        <v>47505</v>
+      </c>
+      <c r="O25">
+        <v>1</v>
+      </c>
+      <c r="W25">
+        <v>47505</v>
+      </c>
+      <c r="X25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>47741</v>
       </c>
@@ -1048,8 +1490,20 @@
       <c r="F26">
         <v>2</v>
       </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="N26">
+        <v>47741</v>
+      </c>
+      <c r="O26">
+        <v>1</v>
+      </c>
+      <c r="W26">
+        <v>47741</v>
+      </c>
+      <c r="X26">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>51013</v>
       </c>
@@ -1068,8 +1522,20 @@
       <c r="F27">
         <v>2</v>
       </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="N27">
+        <v>51013</v>
+      </c>
+      <c r="O27">
+        <v>0</v>
+      </c>
+      <c r="W27">
+        <v>51013</v>
+      </c>
+      <c r="X27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>52073</v>
       </c>
@@ -1088,8 +1554,20 @@
       <c r="F28">
         <v>3</v>
       </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="N28">
+        <v>52073</v>
+      </c>
+      <c r="O28">
+        <v>0</v>
+      </c>
+      <c r="W28">
+        <v>52073</v>
+      </c>
+      <c r="X28">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>55085</v>
       </c>
@@ -1100,7 +1578,7 @@
         <v>1</v>
       </c>
       <c r="D29">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E29">
         <v>4</v>
@@ -1108,8 +1586,20 @@
       <c r="F29">
         <v>4</v>
       </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="N29">
+        <v>55085</v>
+      </c>
+      <c r="O29">
+        <v>0</v>
+      </c>
+      <c r="W29">
+        <v>55085</v>
+      </c>
+      <c r="X29">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>56397</v>
       </c>
@@ -1128,8 +1618,20 @@
       <c r="F30">
         <v>2</v>
       </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="N30">
+        <v>56397</v>
+      </c>
+      <c r="O30">
+        <v>0</v>
+      </c>
+      <c r="W30">
+        <v>56397</v>
+      </c>
+      <c r="X30">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>58245</v>
       </c>
@@ -1148,8 +1650,20 @@
       <c r="F31">
         <v>2</v>
       </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="N31">
+        <v>58245</v>
+      </c>
+      <c r="O31">
+        <v>1</v>
+      </c>
+      <c r="W31">
+        <v>58245</v>
+      </c>
+      <c r="X31">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>59425</v>
       </c>
@@ -1168,8 +1682,20 @@
       <c r="F32">
         <v>4</v>
       </c>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="N32">
+        <v>59425</v>
+      </c>
+      <c r="O32">
+        <v>1</v>
+      </c>
+      <c r="W32">
+        <v>59425</v>
+      </c>
+      <c r="X32">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>62109</v>
       </c>
@@ -1188,8 +1714,20 @@
       <c r="F33">
         <v>4</v>
       </c>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="N33">
+        <v>62109</v>
+      </c>
+      <c r="O33">
+        <v>1</v>
+      </c>
+      <c r="W33">
+        <v>62109</v>
+      </c>
+      <c r="X33">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>64865</v>
       </c>
@@ -1200,7 +1738,7 @@
         <v>1</v>
       </c>
       <c r="D34">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E34">
         <v>4</v>
@@ -1208,8 +1746,20 @@
       <c r="F34">
         <v>2</v>
       </c>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="N34">
+        <v>64865</v>
+      </c>
+      <c r="O34">
+        <v>1</v>
+      </c>
+      <c r="W34">
+        <v>64865</v>
+      </c>
+      <c r="X34">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>65333</v>
       </c>
@@ -1228,8 +1778,20 @@
       <c r="F35">
         <v>5</v>
       </c>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="N35">
+        <v>65333</v>
+      </c>
+      <c r="O35">
+        <v>1</v>
+      </c>
+      <c r="W35">
+        <v>65333</v>
+      </c>
+      <c r="X35">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>65941</v>
       </c>
@@ -1248,8 +1810,20 @@
       <c r="F36">
         <v>1</v>
       </c>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="N36">
+        <v>65941</v>
+      </c>
+      <c r="O36">
+        <v>0</v>
+      </c>
+      <c r="W36">
+        <v>65941</v>
+      </c>
+      <c r="X36">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>67905</v>
       </c>
@@ -1268,8 +1842,20 @@
       <c r="F37">
         <v>2</v>
       </c>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="N37">
+        <v>67905</v>
+      </c>
+      <c r="O37">
+        <v>0</v>
+      </c>
+      <c r="W37">
+        <v>67905</v>
+      </c>
+      <c r="X37">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>69553</v>
       </c>
@@ -1280,7 +1866,7 @@
         <v>1</v>
       </c>
       <c r="D38">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E38">
         <v>2</v>
@@ -1288,8 +1874,20 @@
       <c r="F38">
         <v>4</v>
       </c>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="N38">
+        <v>69553</v>
+      </c>
+      <c r="O38">
+        <v>1</v>
+      </c>
+      <c r="W38">
+        <v>69553</v>
+      </c>
+      <c r="X38">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>70729</v>
       </c>
@@ -1308,8 +1906,20 @@
       <c r="F39">
         <v>1</v>
       </c>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="N39">
+        <v>70729</v>
+      </c>
+      <c r="O39">
+        <v>1</v>
+      </c>
+      <c r="W39">
+        <v>70729</v>
+      </c>
+      <c r="X39">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>71129</v>
       </c>
@@ -1328,8 +1938,20 @@
       <c r="F40">
         <v>2</v>
       </c>
-    </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="N40">
+        <v>71129</v>
+      </c>
+      <c r="O40">
+        <v>0</v>
+      </c>
+      <c r="W40">
+        <v>71129</v>
+      </c>
+      <c r="X40">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>72049</v>
       </c>
@@ -1348,8 +1970,20 @@
       <c r="F41">
         <v>4</v>
       </c>
-    </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="N41">
+        <v>72049</v>
+      </c>
+      <c r="O41">
+        <v>1</v>
+      </c>
+      <c r="W41">
+        <v>72049</v>
+      </c>
+      <c r="X41">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>72257</v>
       </c>
@@ -1368,8 +2002,20 @@
       <c r="F42">
         <v>2</v>
       </c>
-    </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="N42">
+        <v>72257</v>
+      </c>
+      <c r="O42">
+        <v>1</v>
+      </c>
+      <c r="W42">
+        <v>72257</v>
+      </c>
+      <c r="X42">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>72941</v>
       </c>
@@ -1388,8 +2034,20 @@
       <c r="F43">
         <v>3</v>
       </c>
-    </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="N43">
+        <v>72941</v>
+      </c>
+      <c r="O43">
+        <v>1</v>
+      </c>
+      <c r="W43">
+        <v>72941</v>
+      </c>
+      <c r="X43">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>72957</v>
       </c>
@@ -1408,8 +2066,20 @@
       <c r="F44">
         <v>5</v>
       </c>
-    </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="N44">
+        <v>72957</v>
+      </c>
+      <c r="O44">
+        <v>1</v>
+      </c>
+      <c r="W44">
+        <v>72957</v>
+      </c>
+      <c r="X44">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>74773</v>
       </c>
@@ -1428,8 +2098,20 @@
       <c r="F45">
         <v>2</v>
       </c>
-    </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="N45">
+        <v>74773</v>
+      </c>
+      <c r="O45">
+        <v>1</v>
+      </c>
+      <c r="W45">
+        <v>74773</v>
+      </c>
+      <c r="X45">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>77297</v>
       </c>
@@ -1448,8 +2130,20 @@
       <c r="F46">
         <v>5</v>
       </c>
-    </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="N46">
+        <v>77297</v>
+      </c>
+      <c r="O46">
+        <v>1</v>
+      </c>
+      <c r="W46">
+        <v>77297</v>
+      </c>
+      <c r="X46">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>78505</v>
       </c>
@@ -1468,8 +2162,20 @@
       <c r="F47">
         <v>5</v>
       </c>
-    </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="N47">
+        <v>78505</v>
+      </c>
+      <c r="O47">
+        <v>1</v>
+      </c>
+      <c r="W47">
+        <v>78505</v>
+      </c>
+      <c r="X47">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>80329</v>
       </c>
@@ -1488,8 +2194,20 @@
       <c r="F48">
         <v>4</v>
       </c>
-    </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="N48">
+        <v>80329</v>
+      </c>
+      <c r="O48">
+        <v>1</v>
+      </c>
+      <c r="W48">
+        <v>80329</v>
+      </c>
+      <c r="X48">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="49" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>81973</v>
       </c>
@@ -1508,8 +2226,20 @@
       <c r="F49">
         <v>3</v>
       </c>
-    </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="N49">
+        <v>81973</v>
+      </c>
+      <c r="O49">
+        <v>1</v>
+      </c>
+      <c r="W49">
+        <v>81973</v>
+      </c>
+      <c r="X49">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="50" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>84497</v>
       </c>
@@ -1528,8 +2258,20 @@
       <c r="F50">
         <v>1</v>
       </c>
-    </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="N50">
+        <v>84497</v>
+      </c>
+      <c r="O50">
+        <v>1</v>
+      </c>
+      <c r="W50">
+        <v>84497</v>
+      </c>
+      <c r="X50">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>87233</v>
       </c>
@@ -1540,7 +2282,7 @@
         <v>1</v>
       </c>
       <c r="D51">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E51">
         <v>1</v>
@@ -1548,8 +2290,20 @@
       <c r="F51">
         <v>1</v>
       </c>
-    </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="N51">
+        <v>87233</v>
+      </c>
+      <c r="O51">
+        <v>0</v>
+      </c>
+      <c r="W51">
+        <v>87233</v>
+      </c>
+      <c r="X51">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="52" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>89897</v>
       </c>
@@ -1568,8 +2322,20 @@
       <c r="F52">
         <v>3</v>
       </c>
-    </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="N52">
+        <v>89897</v>
+      </c>
+      <c r="O52">
+        <v>0</v>
+      </c>
+      <c r="W52">
+        <v>89897</v>
+      </c>
+      <c r="X52">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>90061</v>
       </c>
@@ -1588,8 +2354,20 @@
       <c r="F53">
         <v>5</v>
       </c>
-    </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="N53">
+        <v>90061</v>
+      </c>
+      <c r="O53">
+        <v>1</v>
+      </c>
+      <c r="W53">
+        <v>90061</v>
+      </c>
+      <c r="X53">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="54" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>93589</v>
       </c>
@@ -1600,7 +2378,7 @@
         <v>1</v>
       </c>
       <c r="D54">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E54">
         <v>4</v>
@@ -1608,8 +2386,20 @@
       <c r="F54">
         <v>5</v>
       </c>
-    </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="N54">
+        <v>93589</v>
+      </c>
+      <c r="O54">
+        <v>0</v>
+      </c>
+      <c r="W54">
+        <v>93589</v>
+      </c>
+      <c r="X54">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="55" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>94077</v>
       </c>
@@ -1628,8 +2418,20 @@
       <c r="F55">
         <v>5</v>
       </c>
-    </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="N55">
+        <v>94077</v>
+      </c>
+      <c r="O55">
+        <v>1</v>
+      </c>
+      <c r="W55">
+        <v>94077</v>
+      </c>
+      <c r="X55">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="56" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>94473</v>
       </c>
@@ -1648,8 +2450,20 @@
       <c r="F56">
         <v>2</v>
       </c>
-    </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="N56">
+        <v>94473</v>
+      </c>
+      <c r="O56">
+        <v>0</v>
+      </c>
+      <c r="W56">
+        <v>94473</v>
+      </c>
+      <c r="X56">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>94893</v>
       </c>
@@ -1668,8 +2482,20 @@
       <c r="F57">
         <v>5</v>
       </c>
-    </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="N57">
+        <v>94893</v>
+      </c>
+      <c r="O57">
+        <v>1</v>
+      </c>
+      <c r="W57">
+        <v>94893</v>
+      </c>
+      <c r="X57">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="58" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>96981</v>
       </c>
@@ -1688,8 +2514,20 @@
       <c r="F58">
         <v>5</v>
       </c>
-    </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="N58">
+        <v>96981</v>
+      </c>
+      <c r="O58">
+        <v>1</v>
+      </c>
+      <c r="W58">
+        <v>96981</v>
+      </c>
+      <c r="X58">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="59" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>98709</v>
       </c>
@@ -1708,8 +2546,20 @@
       <c r="F59">
         <v>1</v>
       </c>
-    </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="N59">
+        <v>98709</v>
+      </c>
+      <c r="O59">
+        <v>1</v>
+      </c>
+      <c r="W59">
+        <v>98709</v>
+      </c>
+      <c r="X59">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>99297</v>
       </c>
@@ -1720,7 +2570,7 @@
         <v>0</v>
       </c>
       <c r="D60">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E60">
         <v>5</v>
@@ -1728,8 +2578,20 @@
       <c r="F60">
         <v>2</v>
       </c>
-    </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="N60">
+        <v>99297</v>
+      </c>
+      <c r="O60">
+        <v>1</v>
+      </c>
+      <c r="W60">
+        <v>99297</v>
+      </c>
+      <c r="X60">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>99585</v>
       </c>
@@ -1748,8 +2610,20 @@
       <c r="F61">
         <v>4</v>
       </c>
-    </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="N61">
+        <v>99585</v>
+      </c>
+      <c r="O61">
+        <v>1</v>
+      </c>
+      <c r="W61">
+        <v>99585</v>
+      </c>
+      <c r="X61">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="62" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>101737</v>
       </c>
@@ -1768,8 +2642,20 @@
       <c r="F62">
         <v>1</v>
       </c>
-    </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="N62">
+        <v>101737</v>
+      </c>
+      <c r="O62">
+        <v>0</v>
+      </c>
+      <c r="W62">
+        <v>101737</v>
+      </c>
+      <c r="X62">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>102013</v>
       </c>
@@ -1788,8 +2674,20 @@
       <c r="F63">
         <v>1</v>
       </c>
-    </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="N63">
+        <v>102013</v>
+      </c>
+      <c r="O63">
+        <v>1</v>
+      </c>
+      <c r="W63">
+        <v>102013</v>
+      </c>
+      <c r="X63">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="64" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>102513</v>
       </c>
@@ -1808,8 +2706,20 @@
       <c r="F64">
         <v>2</v>
       </c>
-    </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="N64">
+        <v>102513</v>
+      </c>
+      <c r="O64">
+        <v>0</v>
+      </c>
+      <c r="W64">
+        <v>102513</v>
+      </c>
+      <c r="X64">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="65" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A65">
         <v>102625</v>
       </c>
@@ -1828,8 +2738,20 @@
       <c r="F65">
         <v>0</v>
       </c>
-    </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="N65">
+        <v>102625</v>
+      </c>
+      <c r="O65">
+        <v>0</v>
+      </c>
+      <c r="W65">
+        <v>102625</v>
+      </c>
+      <c r="X65">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="66" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A66">
         <v>108337</v>
       </c>
@@ -1848,8 +2770,20 @@
       <c r="F66">
         <v>2</v>
       </c>
-    </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="N66">
+        <v>108337</v>
+      </c>
+      <c r="O66">
+        <v>1</v>
+      </c>
+      <c r="W66">
+        <v>108337</v>
+      </c>
+      <c r="X66">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="67" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A67">
         <v>108449</v>
       </c>
@@ -1868,8 +2802,20 @@
       <c r="F67">
         <v>2</v>
       </c>
-    </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="N67">
+        <v>108449</v>
+      </c>
+      <c r="O67">
+        <v>1</v>
+      </c>
+      <c r="W67">
+        <v>108449</v>
+      </c>
+      <c r="X67">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="68" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A68">
         <v>113593</v>
       </c>
@@ -1888,8 +2834,20 @@
       <c r="F68">
         <v>5</v>
       </c>
-    </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="N68">
+        <v>113593</v>
+      </c>
+      <c r="O68">
+        <v>1</v>
+      </c>
+      <c r="W68">
+        <v>113593</v>
+      </c>
+      <c r="X68">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="69" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A69">
         <v>117457</v>
       </c>
@@ -1908,8 +2866,20 @@
       <c r="F69">
         <v>3</v>
       </c>
-    </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="N69">
+        <v>117457</v>
+      </c>
+      <c r="O69">
+        <v>0</v>
+      </c>
+      <c r="W69">
+        <v>117457</v>
+      </c>
+      <c r="X69">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="70" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A70">
         <v>117641</v>
       </c>
@@ -1920,7 +2890,7 @@
         <v>1</v>
       </c>
       <c r="D70">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E70">
         <v>5</v>
@@ -1928,8 +2898,20 @@
       <c r="F70">
         <v>2</v>
       </c>
-    </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="N70">
+        <v>117641</v>
+      </c>
+      <c r="O70">
+        <v>1</v>
+      </c>
+      <c r="W70">
+        <v>117641</v>
+      </c>
+      <c r="X70">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="71" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A71">
         <v>120353</v>
       </c>
@@ -1940,7 +2922,7 @@
         <v>0</v>
       </c>
       <c r="D71">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E71">
         <v>2</v>
@@ -1948,8 +2930,20 @@
       <c r="F71">
         <v>2</v>
       </c>
-    </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="N71">
+        <v>120353</v>
+      </c>
+      <c r="O71">
+        <v>1</v>
+      </c>
+      <c r="W71">
+        <v>120353</v>
+      </c>
+      <c r="X71">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="72" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A72">
         <v>121029</v>
       </c>
@@ -1968,8 +2962,20 @@
       <c r="F72">
         <v>2</v>
       </c>
-    </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="N72">
+        <v>121029</v>
+      </c>
+      <c r="O72">
+        <v>0</v>
+      </c>
+      <c r="W72">
+        <v>121029</v>
+      </c>
+      <c r="X72">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="73" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A73">
         <v>122361</v>
       </c>
@@ -1988,8 +2994,20 @@
       <c r="F73">
         <v>5</v>
       </c>
-    </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="N73">
+        <v>122361</v>
+      </c>
+      <c r="O73">
+        <v>1</v>
+      </c>
+      <c r="W73">
+        <v>122361</v>
+      </c>
+      <c r="X73">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="74" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A74">
         <v>128045</v>
       </c>
@@ -2008,8 +3026,20 @@
       <c r="F74">
         <v>4</v>
       </c>
-    </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="N74">
+        <v>128045</v>
+      </c>
+      <c r="O74">
+        <v>1</v>
+      </c>
+      <c r="W74">
+        <v>128045</v>
+      </c>
+      <c r="X74">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="75" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A75">
         <v>128581</v>
       </c>
@@ -2028,8 +3058,20 @@
       <c r="F75">
         <v>3</v>
       </c>
-    </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="N75">
+        <v>128581</v>
+      </c>
+      <c r="O75">
+        <v>1</v>
+      </c>
+      <c r="W75">
+        <v>128581</v>
+      </c>
+      <c r="X75">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="76" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A76">
         <v>129885</v>
       </c>
@@ -2048,8 +3090,20 @@
       <c r="F76">
         <v>1</v>
       </c>
-    </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="N76">
+        <v>129885</v>
+      </c>
+      <c r="O76">
+        <v>1</v>
+      </c>
+      <c r="W76">
+        <v>129885</v>
+      </c>
+      <c r="X76">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="77" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A77">
         <v>130065</v>
       </c>
@@ -2068,8 +3122,20 @@
       <c r="F77">
         <v>4</v>
       </c>
-    </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="N77">
+        <v>130065</v>
+      </c>
+      <c r="O77">
+        <v>1</v>
+      </c>
+      <c r="W77">
+        <v>130065</v>
+      </c>
+      <c r="X77">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="78" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A78">
         <v>131913</v>
       </c>
@@ -2088,8 +3154,20 @@
       <c r="F78">
         <v>2</v>
       </c>
-    </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="N78">
+        <v>131913</v>
+      </c>
+      <c r="O78">
+        <v>0</v>
+      </c>
+      <c r="W78">
+        <v>131913</v>
+      </c>
+      <c r="X78">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="79" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A79">
         <v>133477</v>
       </c>
@@ -2108,8 +3186,20 @@
       <c r="F79">
         <v>2</v>
       </c>
-    </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="N79">
+        <v>133477</v>
+      </c>
+      <c r="O79">
+        <v>0</v>
+      </c>
+      <c r="W79">
+        <v>133477</v>
+      </c>
+      <c r="X79">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="80" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A80">
         <v>133889</v>
       </c>
@@ -2128,8 +3218,20 @@
       <c r="F80">
         <v>1</v>
       </c>
-    </row>
-    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="N80">
+        <v>133889</v>
+      </c>
+      <c r="O80">
+        <v>0</v>
+      </c>
+      <c r="W80">
+        <v>133889</v>
+      </c>
+      <c r="X80">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="81" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A81">
         <v>136097</v>
       </c>
@@ -2148,8 +3250,20 @@
       <c r="F81">
         <v>3</v>
       </c>
-    </row>
-    <row r="82" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="N81">
+        <v>136097</v>
+      </c>
+      <c r="O81">
+        <v>1</v>
+      </c>
+      <c r="W81">
+        <v>136097</v>
+      </c>
+      <c r="X81">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="82" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A82">
         <v>138201</v>
       </c>
@@ -2168,8 +3282,20 @@
       <c r="F82">
         <v>2</v>
       </c>
-    </row>
-    <row r="83" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="N82">
+        <v>138201</v>
+      </c>
+      <c r="O82">
+        <v>1</v>
+      </c>
+      <c r="W82">
+        <v>138201</v>
+      </c>
+      <c r="X82">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="83" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A83">
         <v>140529</v>
       </c>
@@ -2188,8 +3314,20 @@
       <c r="F83">
         <v>2</v>
       </c>
-    </row>
-    <row r="84" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="N83">
+        <v>140529</v>
+      </c>
+      <c r="O83">
+        <v>0</v>
+      </c>
+      <c r="W83">
+        <v>140529</v>
+      </c>
+      <c r="X83">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="84" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A84">
         <v>142029</v>
       </c>
@@ -2208,8 +3346,20 @@
       <c r="F84">
         <v>1</v>
       </c>
-    </row>
-    <row r="85" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="N84">
+        <v>142029</v>
+      </c>
+      <c r="O84">
+        <v>0</v>
+      </c>
+      <c r="W84">
+        <v>142029</v>
+      </c>
+      <c r="X84">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="85" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A85">
         <v>142073</v>
       </c>
@@ -2228,8 +3378,20 @@
       <c r="F85">
         <v>4</v>
       </c>
-    </row>
-    <row r="86" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="N85">
+        <v>142073</v>
+      </c>
+      <c r="O85">
+        <v>1</v>
+      </c>
+      <c r="W85">
+        <v>142073</v>
+      </c>
+      <c r="X85">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="86" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A86">
         <v>142993</v>
       </c>
@@ -2248,8 +3410,20 @@
       <c r="F86">
         <v>1</v>
       </c>
-    </row>
-    <row r="87" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="N86">
+        <v>142993</v>
+      </c>
+      <c r="O86">
+        <v>1</v>
+      </c>
+      <c r="W86">
+        <v>142993</v>
+      </c>
+      <c r="X86">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="87" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A87">
         <v>144489</v>
       </c>
@@ -2268,8 +3442,20 @@
       <c r="F87">
         <v>1</v>
       </c>
-    </row>
-    <row r="88" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="N87">
+        <v>144489</v>
+      </c>
+      <c r="O87">
+        <v>0</v>
+      </c>
+      <c r="W87">
+        <v>144489</v>
+      </c>
+      <c r="X87">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="88" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A88">
         <v>150549</v>
       </c>
@@ -2288,8 +3474,20 @@
       <c r="F88">
         <v>2</v>
       </c>
-    </row>
-    <row r="89" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="N88">
+        <v>150549</v>
+      </c>
+      <c r="O88">
+        <v>0</v>
+      </c>
+      <c r="W88">
+        <v>150549</v>
+      </c>
+      <c r="X88">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="89" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A89">
         <v>151293</v>
       </c>
@@ -2308,8 +3506,20 @@
       <c r="F89">
         <v>3</v>
       </c>
-    </row>
-    <row r="90" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="N89">
+        <v>151293</v>
+      </c>
+      <c r="O89">
+        <v>0</v>
+      </c>
+      <c r="W89">
+        <v>151293</v>
+      </c>
+      <c r="X89">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="90" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A90">
         <v>155089</v>
       </c>
@@ -2328,8 +3538,20 @@
       <c r="F90">
         <v>5</v>
       </c>
-    </row>
-    <row r="91" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="N90">
+        <v>155089</v>
+      </c>
+      <c r="O90">
+        <v>1</v>
+      </c>
+      <c r="W90">
+        <v>155089</v>
+      </c>
+      <c r="X90">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="91" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A91">
         <v>157069</v>
       </c>
@@ -2348,8 +3570,20 @@
       <c r="F91">
         <v>2</v>
       </c>
-    </row>
-    <row r="92" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="N91">
+        <v>157069</v>
+      </c>
+      <c r="O91">
+        <v>1</v>
+      </c>
+      <c r="W91">
+        <v>157069</v>
+      </c>
+      <c r="X91">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="92" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A92">
         <v>157209</v>
       </c>
@@ -2368,8 +3602,20 @@
       <c r="F92">
         <v>1</v>
       </c>
-    </row>
-    <row r="93" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="N92">
+        <v>157209</v>
+      </c>
+      <c r="O92">
+        <v>0</v>
+      </c>
+      <c r="W92">
+        <v>157209</v>
+      </c>
+      <c r="X92">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="93" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A93">
         <v>159273</v>
       </c>
@@ -2388,8 +3634,20 @@
       <c r="F93">
         <v>1</v>
       </c>
-    </row>
-    <row r="94" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="N93">
+        <v>159273</v>
+      </c>
+      <c r="O93">
+        <v>0</v>
+      </c>
+      <c r="W93">
+        <v>159273</v>
+      </c>
+      <c r="X93">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="94" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A94">
         <v>161113</v>
       </c>
@@ -2408,8 +3666,20 @@
       <c r="F94">
         <v>2</v>
       </c>
-    </row>
-    <row r="95" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="N94">
+        <v>161113</v>
+      </c>
+      <c r="O94">
+        <v>0</v>
+      </c>
+      <c r="W94">
+        <v>161113</v>
+      </c>
+      <c r="X94">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="95" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A95">
         <v>161237</v>
       </c>
@@ -2428,8 +3698,20 @@
       <c r="F95">
         <v>5</v>
       </c>
-    </row>
-    <row r="96" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="N95">
+        <v>161237</v>
+      </c>
+      <c r="O95">
+        <v>1</v>
+      </c>
+      <c r="W95">
+        <v>161237</v>
+      </c>
+      <c r="X95">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="96" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A96">
         <v>162265</v>
       </c>
@@ -2448,8 +3730,20 @@
       <c r="F96">
         <v>2</v>
       </c>
-    </row>
-    <row r="97" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="N96">
+        <v>162265</v>
+      </c>
+      <c r="O96">
+        <v>0</v>
+      </c>
+      <c r="W96">
+        <v>162265</v>
+      </c>
+      <c r="X96">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="97" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A97">
         <v>171017</v>
       </c>
@@ -2468,8 +3762,20 @@
       <c r="F97">
         <v>4</v>
       </c>
-    </row>
-    <row r="98" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="N97">
+        <v>171017</v>
+      </c>
+      <c r="O97">
+        <v>1</v>
+      </c>
+      <c r="W97">
+        <v>171017</v>
+      </c>
+      <c r="X97">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="98" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A98">
         <v>171465</v>
       </c>
@@ -2488,8 +3794,20 @@
       <c r="F98">
         <v>2</v>
       </c>
-    </row>
-    <row r="99" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="N98">
+        <v>171465</v>
+      </c>
+      <c r="O98">
+        <v>0</v>
+      </c>
+      <c r="W98">
+        <v>171465</v>
+      </c>
+      <c r="X98">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="99" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A99">
         <v>174289</v>
       </c>
@@ -2508,8 +3826,20 @@
       <c r="F99">
         <v>1</v>
       </c>
-    </row>
-    <row r="100" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="N99">
+        <v>174289</v>
+      </c>
+      <c r="O99">
+        <v>0</v>
+      </c>
+      <c r="W99">
+        <v>174289</v>
+      </c>
+      <c r="X99">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="100" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A100">
         <v>176157</v>
       </c>
@@ -2528,8 +3858,20 @@
       <c r="F100">
         <v>1</v>
       </c>
-    </row>
-    <row r="101" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="N100">
+        <v>176157</v>
+      </c>
+      <c r="O100">
+        <v>0</v>
+      </c>
+      <c r="W100">
+        <v>176157</v>
+      </c>
+      <c r="X100">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="101" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A101">
         <v>176189</v>
       </c>
@@ -2548,8 +3890,20 @@
       <c r="F101">
         <v>2</v>
       </c>
-    </row>
-    <row r="102" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="N101">
+        <v>176189</v>
+      </c>
+      <c r="O101">
+        <v>0</v>
+      </c>
+      <c r="W101">
+        <v>176189</v>
+      </c>
+      <c r="X101">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="102" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A102">
         <v>176329</v>
       </c>
@@ -2568,8 +3922,24 @@
       <c r="F102">
         <v>5</v>
       </c>
+      <c r="N102">
+        <v>176329</v>
+      </c>
+      <c r="O102">
+        <v>1</v>
+      </c>
+      <c r="W102">
+        <v>176329</v>
+      </c>
+      <c r="X102">
+        <v>1</v>
+      </c>
     </row>
   </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="O1:Q1"/>
+    <mergeCell ref="X1:Z1"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>